<commit_message>
decomposing notebooks into dcca mapping, land use and prevalence investigation
</commit_message>
<xml_diff>
--- a/ha_dcca03_dict.xlsx
+++ b/ha_dcca03_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Districtname</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>district</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -467,6 +472,11 @@
           <t>['ADMIRALTY', 'CENTRAL']</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ADMIRALTY</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -485,6 +495,11 @@
           <t>['GREEN ISLAND', 'MOUNT DAVIS']</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>GREEN ISLAND</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -503,6 +518,11 @@
           <t>['CYBER PORT', 'POKFULAM', 'SANDY BAY']</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CYBER PORT</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -521,6 +541,11 @@
           <t>['CHUNG HOM KOK', 'DEEP WATER BAY', 'NAM LONG SHAN', 'REPULSE BAY', 'SHOUSON HILL']</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CHUNG HOM KOK</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -539,6 +564,11 @@
           <t>['SHEK O', 'STANLEY', 'TAI TAM']</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SHEK O</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -557,6 +587,11 @@
           <t>['LEI YUE MUN', 'YAU TONG']</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LEI YUE MUN</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -575,6 +610,11 @@
           <t>['SHAM TSENG', 'TING KAU']</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SHAM TSENG</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -593,6 +633,11 @@
           <t>['SIU LAM', 'TAI LAM CHUNG']</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SIU LAM</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -611,6 +656,11 @@
           <t>['LUNG KWU TAN', 'NIM WAN', 'TAP SHEK KOK']</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LUNG KWU TAN</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -629,6 +679,11 @@
           <t>['LAM TEI', 'NAI WAI', 'YICK YUEN']</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LAM TEI</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -647,6 +702,11 @@
           <t>['MAI PO', 'NAM SANG WAI', 'NGAU TAM MEI', 'SUN TIN']</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>MAI PO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -665,6 +725,11 @@
           <t>['CLOSED AREA', 'HUNG LUNG HANG', 'LUK KENG', 'NAM CHUNG', 'SHA TAU KOK', 'TA KWU LING']</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CLOSED AREA</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -683,6 +748,11 @@
           <t>['FEI NGO SHAN', 'HO CHUNG KUK']</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>FEI NGO SHAN</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -701,6 +771,11 @@
           <t>['KAU SAI CHAU', 'TAI MONG TSAI']</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>KAU SAI CHAU</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -719,6 +794,11 @@
           <t>['CLEAR WATER BAY', 'SILVERSTRAND']</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CLEAR WATER BAY</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -737,6 +817,11 @@
           <t>['CHI MA WAN', 'LANTAU ISLAND', 'MUI WO', 'NGONG PING', 'SHA LO WAN', 'SHAM WAT', 'SHEK KWU CHAU', 'SOKO ISLANDS', 'TAI O']</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CHI MA WAN</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -755,6 +840,11 @@
           <t>['HEI LING CHAU', 'PENG CHAU']</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>HEI LING CHAU</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -771,6 +861,11 @@
       <c r="D19" t="inlineStr">
         <is>
           <t>['LAMMA ISLAND', 'PO TOI ISLANDS']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LAMMA ISLAND</t>
         </is>
       </c>
     </row>

</xml_diff>